<commit_message>
Home Screen test cases are added
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Profile.xlsx
+++ b/bin/com/NFHS/xls/Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17610" windowHeight="3855" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17610" windowHeight="3855" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>bhabani.shankar105@weboapps.com</t>
-  </si>
-  <si>
-    <t>test1234</t>
-  </si>
-  <si>
     <t>MA_AccountEdit1</t>
   </si>
   <si>
@@ -61,12 +55,25 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>admin@nfhslearn.com</t>
+  </si>
+  <si>
+    <t>nfhslearn@6186</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -440,17 +447,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="55.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1">
@@ -475,16 +482,19 @@
     </row>
     <row r="2" spans="1:6" ht="82.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -527,16 +537,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -558,19 +568,22 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored Test cases for Home Screen Messages and Slider Tool
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Profile.xlsx
+++ b/bin/com/NFHS/xls/Profile.xlsx
@@ -4,18 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17610" windowHeight="3855" tabRatio="883"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17610" windowHeight="3855" tabRatio="883" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="MA_AccountEdit1" sheetId="2" r:id="rId2"/>
+    <sheet name="MA_FulfillmentTool" sheetId="3" r:id="rId3"/>
+    <sheet name="HomeScreen1" sheetId="4" r:id="rId4"/>
+    <sheet name="HomeScreen2" sheetId="5" r:id="rId5"/>
+    <sheet name="HomeScreen3" sheetId="6" r:id="rId6"/>
+    <sheet name="SlideTool1" sheetId="7" r:id="rId7"/>
+    <sheet name="SlideTool2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>TCID</t>
   </si>
@@ -51,9 +57,6 @@
     <t>MA_AccountEdit1</t>
   </si>
   <si>
-    <t>exected</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -66,14 +69,35 @@
     <t>pass</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>MA_FulfillmentTool</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>HomeScreen3</t>
+  </si>
+  <si>
+    <t>HomeScreen1</t>
+  </si>
+  <si>
+    <t>HomeScreen2</t>
+  </si>
+  <si>
+    <t>SlideTool1</t>
+  </si>
+  <si>
+    <t>SlideTool2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -445,19 +469,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="55.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1">
@@ -488,44 +512,82 @@
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="103.5" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -538,15 +600,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="1" max="1" width="38.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -568,17 +630,373 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="57.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>